<commit_message>
Implement semi-magic detection and behavior
</commit_message>
<xml_diff>
--- a/examples/magic-checker.xlsx
+++ b/examples/magic-checker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lioudt/Documents/Projects/Albrecht/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B751D3E-5E9F-C243-8B89-D05ED6564467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A66291D7-01EF-7E42-9D39-B814EB7F32BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{88018936-75B0-5E47-B04F-69E20E6F83B4}"/>
+    <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{88018936-75B0-5E47-B04F-69E20E6F83B4}"/>
   </bookViews>
   <sheets>
     <sheet name="9" sheetId="1" r:id="rId1"/>
@@ -444,7 +444,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D268AA-9B72-C74E-AFE5-98BDA6ADCB5F}">
   <dimension ref="A1:K10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:J9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -801,6 +803,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -808,102 +811,100 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E8CD7C-B77D-014B-894F-5F39F26D2D1B}">
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B1">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="C1">
-        <v>428</v>
+        <v>630</v>
       </c>
       <c r="D1">
         <v>518</v>
       </c>
       <c r="E1">
-        <v>863</v>
+        <v>331</v>
       </c>
       <c r="F1">
-        <v>793</v>
+        <v>598</v>
       </c>
       <c r="G1">
-        <v>727</v>
+        <v>608</v>
       </c>
       <c r="H1">
-        <v>656</v>
+        <v>147</v>
       </c>
       <c r="I1">
-        <v>384</v>
+        <v>291</v>
       </c>
       <c r="J1">
-        <v>250</v>
+        <v>507</v>
       </c>
       <c r="K1">
-        <v>618</v>
+        <v>282</v>
       </c>
       <c r="L1">
-        <v>866</v>
+        <v>445</v>
       </c>
       <c r="M1">
-        <v>187</v>
+        <v>729</v>
       </c>
       <c r="N1">
-        <v>80</v>
+        <v>830</v>
       </c>
       <c r="O1">
-        <v>448</v>
+        <v>150</v>
       </c>
       <c r="P1">
-        <v>582</v>
+        <v>617</v>
       </c>
       <c r="Q1">
-        <v>107</v>
+        <v>292</v>
       </c>
       <c r="R1">
-        <v>236</v>
+        <v>498</v>
       </c>
       <c r="S1">
-        <v>620</v>
+        <v>323</v>
       </c>
       <c r="T1">
-        <v>195</v>
+        <v>77</v>
       </c>
       <c r="U1">
-        <v>154</v>
+        <v>469</v>
       </c>
       <c r="V1">
-        <v>129</v>
+        <v>813</v>
       </c>
       <c r="W1">
-        <v>878</v>
+        <v>817</v>
       </c>
       <c r="X1">
-        <v>562</v>
+        <v>814</v>
       </c>
       <c r="Y1">
-        <v>851</v>
+        <v>857</v>
       </c>
       <c r="Z1">
-        <v>368</v>
+        <v>177</v>
       </c>
       <c r="AA1">
-        <v>405</v>
+        <v>306</v>
       </c>
       <c r="AB1">
-        <v>323</v>
+        <v>54</v>
       </c>
       <c r="AC1">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="AD1">
-        <v>181</v>
+        <v>551</v>
       </c>
       <c r="AE1">
-        <v>700</v>
+        <v>508</v>
       </c>
       <c r="AF1">
         <f>SUM(B1:AE1)</f>
@@ -912,94 +913,94 @@
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B2">
-        <v>872</v>
+        <v>801</v>
       </c>
       <c r="C2">
-        <v>503</v>
+        <v>821</v>
       </c>
       <c r="D2">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E2">
-        <v>762</v>
+        <v>210</v>
       </c>
       <c r="F2">
-        <v>69</v>
+        <v>654</v>
       </c>
       <c r="G2">
-        <v>275</v>
+        <v>784</v>
       </c>
       <c r="H2">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="I2">
-        <v>7</v>
+        <v>741</v>
       </c>
       <c r="J2">
-        <v>899</v>
+        <v>267</v>
       </c>
       <c r="K2">
-        <v>734</v>
+        <v>893</v>
       </c>
       <c r="L2">
-        <v>613</v>
+        <v>788</v>
       </c>
       <c r="M2">
-        <v>277</v>
+        <v>15</v>
       </c>
       <c r="N2">
-        <v>55</v>
+        <v>316</v>
       </c>
       <c r="O2">
-        <v>610</v>
+        <v>332</v>
       </c>
       <c r="P2">
-        <v>663</v>
+        <v>580</v>
       </c>
       <c r="Q2">
-        <v>544</v>
+        <v>90</v>
       </c>
       <c r="R2">
-        <v>509</v>
+        <v>137</v>
       </c>
       <c r="S2">
-        <v>32</v>
+        <v>796</v>
       </c>
       <c r="T2">
-        <v>642</v>
+        <v>453</v>
       </c>
       <c r="U2">
-        <v>214</v>
+        <v>157</v>
       </c>
       <c r="V2">
-        <v>252</v>
+        <v>183</v>
       </c>
       <c r="W2">
-        <v>769</v>
+        <v>687</v>
       </c>
       <c r="X2">
-        <v>246</v>
+        <v>491</v>
       </c>
       <c r="Y2">
-        <v>258</v>
+        <v>229</v>
       </c>
       <c r="Z2">
-        <v>717</v>
+        <v>255</v>
       </c>
       <c r="AA2">
-        <v>649</v>
+        <v>505</v>
       </c>
       <c r="AB2">
-        <v>876</v>
+        <v>683</v>
       </c>
       <c r="AC2">
-        <v>862</v>
+        <v>387</v>
       </c>
       <c r="AD2">
-        <v>201</v>
+        <v>135</v>
       </c>
       <c r="AE2">
-        <v>66</v>
+        <v>689</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF30" si="0">SUM(B2:AE2)</f>
@@ -1008,94 +1009,94 @@
     </row>
     <row r="3" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B3">
-        <v>354</v>
+        <v>217</v>
       </c>
       <c r="C3">
-        <v>502</v>
+        <v>542</v>
       </c>
       <c r="D3">
-        <v>151</v>
+        <v>708</v>
       </c>
       <c r="E3">
-        <v>896</v>
+        <v>68</v>
       </c>
       <c r="F3">
-        <v>796</v>
+        <v>178</v>
       </c>
       <c r="G3">
-        <v>895</v>
+        <v>239</v>
       </c>
       <c r="H3">
-        <v>499</v>
+        <v>202</v>
       </c>
       <c r="I3">
-        <v>153</v>
+        <v>276</v>
       </c>
       <c r="J3">
-        <v>373</v>
+        <v>405</v>
       </c>
       <c r="K3">
-        <v>437</v>
+        <v>264</v>
       </c>
       <c r="L3">
-        <v>817</v>
+        <v>847</v>
       </c>
       <c r="M3">
-        <v>314</v>
+        <v>673</v>
       </c>
       <c r="N3">
+        <v>874</v>
+      </c>
+      <c r="O3">
+        <v>427</v>
+      </c>
+      <c r="P3">
+        <v>409</v>
+      </c>
+      <c r="Q3">
+        <v>613</v>
+      </c>
+      <c r="R3">
+        <v>717</v>
+      </c>
+      <c r="S3">
+        <v>104</v>
+      </c>
+      <c r="T3">
+        <v>420</v>
+      </c>
+      <c r="U3">
+        <v>285</v>
+      </c>
+      <c r="V3">
+        <v>690</v>
+      </c>
+      <c r="W3">
+        <v>597</v>
+      </c>
+      <c r="X3">
+        <v>168</v>
+      </c>
+      <c r="Y3">
+        <v>811</v>
+      </c>
+      <c r="Z3">
+        <v>313</v>
+      </c>
+      <c r="AA3">
+        <v>62</v>
+      </c>
+      <c r="AB3">
+        <v>820</v>
+      </c>
+      <c r="AC3">
         <v>604</v>
       </c>
-      <c r="O3">
-        <v>10</v>
-      </c>
-      <c r="P3">
-        <v>81</v>
-      </c>
-      <c r="Q3">
-        <v>92</v>
-      </c>
-      <c r="R3">
-        <v>39</v>
-      </c>
-      <c r="S3">
-        <v>892</v>
-      </c>
-      <c r="T3">
-        <v>746</v>
-      </c>
-      <c r="U3">
-        <v>36</v>
-      </c>
-      <c r="V3">
-        <v>97</v>
-      </c>
-      <c r="W3">
-        <v>879</v>
-      </c>
-      <c r="X3">
-        <v>230</v>
-      </c>
-      <c r="Y3">
-        <v>194</v>
-      </c>
-      <c r="Z3">
-        <v>398</v>
-      </c>
-      <c r="AA3">
-        <v>844</v>
-      </c>
-      <c r="AB3">
-        <v>720</v>
-      </c>
-      <c r="AC3">
-        <v>497</v>
-      </c>
       <c r="AD3">
-        <v>764</v>
+        <v>601</v>
       </c>
       <c r="AE3">
-        <v>205</v>
+        <v>381</v>
       </c>
       <c r="AF3">
         <f t="shared" si="0"/>
@@ -1104,94 +1105,94 @@
     </row>
     <row r="4" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B4">
-        <v>161</v>
+        <v>650</v>
       </c>
       <c r="C4">
-        <v>783</v>
+        <v>379</v>
       </c>
       <c r="D4">
-        <v>791</v>
+        <v>806</v>
       </c>
       <c r="E4">
-        <v>87</v>
+        <v>576</v>
       </c>
       <c r="F4">
-        <v>761</v>
+        <v>228</v>
       </c>
       <c r="G4">
-        <v>837</v>
+        <v>281</v>
       </c>
       <c r="H4">
-        <v>310</v>
+        <v>516</v>
       </c>
       <c r="I4">
-        <v>898</v>
+        <v>679</v>
       </c>
       <c r="J4">
-        <v>59</v>
+        <v>765</v>
       </c>
       <c r="K4">
-        <v>134</v>
+        <v>67</v>
       </c>
       <c r="L4">
+        <v>193</v>
+      </c>
+      <c r="M4">
+        <v>56</v>
+      </c>
+      <c r="N4">
+        <v>585</v>
+      </c>
+      <c r="O4">
+        <v>866</v>
+      </c>
+      <c r="P4">
+        <v>506</v>
+      </c>
+      <c r="Q4">
         <v>476</v>
       </c>
-      <c r="M4">
-        <v>719</v>
-      </c>
-      <c r="N4">
-        <v>815</v>
-      </c>
-      <c r="O4">
-        <v>192</v>
-      </c>
-      <c r="P4">
-        <v>282</v>
-      </c>
-      <c r="Q4">
-        <v>757</v>
-      </c>
       <c r="R4">
-        <v>749</v>
+        <v>733</v>
       </c>
       <c r="S4">
-        <v>578</v>
+        <v>248</v>
       </c>
       <c r="T4">
-        <v>227</v>
+        <v>335</v>
       </c>
       <c r="U4">
-        <v>593</v>
+        <v>831</v>
       </c>
       <c r="V4">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="W4">
-        <v>67</v>
+        <v>142</v>
       </c>
       <c r="X4">
-        <v>372</v>
+        <v>230</v>
       </c>
       <c r="Y4">
-        <v>575</v>
+        <v>280</v>
       </c>
       <c r="Z4">
-        <v>272</v>
+        <v>365</v>
       </c>
       <c r="AA4">
-        <v>304</v>
+        <v>881</v>
       </c>
       <c r="AB4">
-        <v>216</v>
+        <v>620</v>
       </c>
       <c r="AC4">
-        <v>24</v>
+        <v>647</v>
       </c>
       <c r="AD4">
-        <v>597</v>
+        <v>204</v>
       </c>
       <c r="AE4">
-        <v>754</v>
+        <v>155</v>
       </c>
       <c r="AF4">
         <f t="shared" si="0"/>
@@ -1200,94 +1201,94 @@
     </row>
     <row r="5" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B5">
-        <v>427</v>
+        <v>390</v>
       </c>
       <c r="C5">
-        <v>306</v>
+        <v>464</v>
       </c>
       <c r="D5">
-        <v>814</v>
+        <v>123</v>
       </c>
       <c r="E5">
-        <v>358</v>
+        <v>19</v>
       </c>
       <c r="F5">
-        <v>4</v>
+        <v>504</v>
       </c>
       <c r="G5">
-        <v>429</v>
+        <v>412</v>
       </c>
       <c r="H5">
-        <v>869</v>
+        <v>860</v>
       </c>
       <c r="I5">
-        <v>471</v>
+        <v>194</v>
       </c>
       <c r="J5">
-        <v>778</v>
+        <v>463</v>
       </c>
       <c r="K5">
-        <v>83</v>
+        <v>170</v>
       </c>
       <c r="L5">
-        <v>99</v>
+        <v>497</v>
       </c>
       <c r="M5">
-        <v>220</v>
+        <v>795</v>
       </c>
       <c r="N5">
-        <v>732</v>
+        <v>11</v>
       </c>
       <c r="O5">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="P5">
-        <v>586</v>
+        <v>661</v>
       </c>
       <c r="Q5">
-        <v>265</v>
+        <v>678</v>
       </c>
       <c r="R5">
-        <v>689</v>
+        <v>593</v>
       </c>
       <c r="S5">
-        <v>722</v>
+        <v>735</v>
       </c>
       <c r="T5">
-        <v>741</v>
+        <v>720</v>
       </c>
       <c r="U5">
-        <v>565</v>
+        <v>271</v>
       </c>
       <c r="V5">
-        <v>77</v>
+        <v>187</v>
       </c>
       <c r="W5">
-        <v>833</v>
+        <v>317</v>
       </c>
       <c r="X5">
-        <v>408</v>
+        <v>45</v>
       </c>
       <c r="Y5">
-        <v>385</v>
+        <v>885</v>
       </c>
       <c r="Z5">
-        <v>200</v>
+        <v>460</v>
       </c>
       <c r="AA5">
-        <v>264</v>
+        <v>798</v>
       </c>
       <c r="AB5">
-        <v>708</v>
+        <v>449</v>
       </c>
       <c r="AC5">
-        <v>301</v>
+        <v>667</v>
       </c>
       <c r="AD5">
-        <v>393</v>
+        <v>421</v>
       </c>
       <c r="AE5">
-        <v>682</v>
+        <v>631</v>
       </c>
       <c r="AF5">
         <f t="shared" si="0"/>
@@ -1296,94 +1297,94 @@
     </row>
     <row r="6" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B6">
-        <v>330</v>
+        <v>47</v>
       </c>
       <c r="C6">
-        <v>886</v>
+        <v>894</v>
       </c>
       <c r="D6">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="E6">
-        <v>155</v>
+        <v>550</v>
       </c>
       <c r="F6">
-        <v>48</v>
+        <v>764</v>
       </c>
       <c r="G6">
-        <v>794</v>
+        <v>304</v>
       </c>
       <c r="H6">
-        <v>72</v>
+        <v>269</v>
       </c>
       <c r="I6">
-        <v>351</v>
+        <v>434</v>
       </c>
       <c r="J6">
-        <v>828</v>
+        <v>320</v>
       </c>
       <c r="K6">
-        <v>415</v>
+        <v>760</v>
       </c>
       <c r="L6">
-        <v>159</v>
+        <v>524</v>
       </c>
       <c r="M6">
-        <v>479</v>
+        <v>86</v>
       </c>
       <c r="N6">
-        <v>371</v>
+        <v>112</v>
       </c>
       <c r="O6">
-        <v>580</v>
+        <v>23</v>
       </c>
       <c r="P6">
-        <v>344</v>
+        <v>106</v>
       </c>
       <c r="Q6">
-        <v>487</v>
+        <v>397</v>
       </c>
       <c r="R6">
-        <v>199</v>
+        <v>864</v>
       </c>
       <c r="S6">
-        <v>631</v>
+        <v>408</v>
       </c>
       <c r="T6">
-        <v>724</v>
+        <v>739</v>
       </c>
       <c r="U6">
-        <v>141</v>
+        <v>433</v>
       </c>
       <c r="V6">
-        <v>690</v>
+        <v>278</v>
       </c>
       <c r="W6">
-        <v>581</v>
+        <v>83</v>
       </c>
       <c r="X6">
-        <v>616</v>
+        <v>859</v>
       </c>
       <c r="Y6">
-        <v>101</v>
+        <v>132</v>
       </c>
       <c r="Z6">
-        <v>877</v>
+        <v>668</v>
       </c>
       <c r="AA6">
-        <v>416</v>
+        <v>578</v>
       </c>
       <c r="AB6">
-        <v>319</v>
+        <v>492</v>
       </c>
       <c r="AC6">
-        <v>266</v>
+        <v>440</v>
       </c>
       <c r="AD6">
-        <v>676</v>
+        <v>666</v>
       </c>
       <c r="AE6">
-        <v>336</v>
+        <v>644</v>
       </c>
       <c r="AF6">
         <f t="shared" si="0"/>
@@ -1392,94 +1393,94 @@
     </row>
     <row r="7" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B7">
-        <v>243</v>
+        <v>870</v>
       </c>
       <c r="C7">
-        <v>127</v>
+        <v>334</v>
       </c>
       <c r="D7">
-        <v>884</v>
+        <v>347</v>
       </c>
       <c r="E7">
-        <v>226</v>
+        <v>315</v>
       </c>
       <c r="F7">
-        <v>95</v>
+        <v>603</v>
       </c>
       <c r="G7">
-        <v>283</v>
+        <v>80</v>
       </c>
       <c r="H7">
-        <v>91</v>
+        <v>290</v>
       </c>
       <c r="I7">
-        <v>215</v>
+        <v>832</v>
       </c>
       <c r="J7">
-        <v>394</v>
+        <v>293</v>
       </c>
       <c r="K7">
-        <v>42</v>
+        <v>794</v>
       </c>
       <c r="L7">
-        <v>489</v>
+        <v>522</v>
       </c>
       <c r="M7">
-        <v>853</v>
+        <v>645</v>
       </c>
       <c r="N7">
-        <v>178</v>
+        <v>681</v>
       </c>
       <c r="O7">
-        <v>369</v>
+        <v>669</v>
       </c>
       <c r="P7">
-        <v>376</v>
+        <v>165</v>
       </c>
       <c r="Q7">
-        <v>785</v>
+        <v>89</v>
       </c>
       <c r="R7">
-        <v>297</v>
+        <v>891</v>
       </c>
       <c r="S7">
-        <v>496</v>
+        <v>198</v>
       </c>
       <c r="T7">
-        <v>449</v>
+        <v>742</v>
       </c>
       <c r="U7">
-        <v>625</v>
+        <v>346</v>
       </c>
       <c r="V7">
-        <v>710</v>
+        <v>701</v>
       </c>
       <c r="W7">
-        <v>303</v>
+        <v>525</v>
       </c>
       <c r="X7">
-        <v>472</v>
+        <v>371</v>
       </c>
       <c r="Y7">
-        <v>473</v>
+        <v>310</v>
       </c>
       <c r="Z7">
-        <v>647</v>
+        <v>477</v>
       </c>
       <c r="AA7">
-        <v>665</v>
+        <v>158</v>
       </c>
       <c r="AB7">
-        <v>466</v>
+        <v>149</v>
       </c>
       <c r="AC7">
-        <v>563</v>
+        <v>792</v>
       </c>
       <c r="AD7">
-        <v>857</v>
+        <v>63</v>
       </c>
       <c r="AE7">
-        <v>842</v>
+        <v>263</v>
       </c>
       <c r="AF7">
         <f t="shared" si="0"/>
@@ -1488,94 +1489,94 @@
     </row>
     <row r="8" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B8">
-        <v>823</v>
+        <v>473</v>
       </c>
       <c r="C8">
-        <v>284</v>
+        <v>44</v>
       </c>
       <c r="D8">
-        <v>452</v>
+        <v>256</v>
       </c>
       <c r="E8">
-        <v>338</v>
+        <v>718</v>
       </c>
       <c r="F8">
-        <v>225</v>
+        <v>336</v>
       </c>
       <c r="G8">
-        <v>548</v>
+        <v>148</v>
       </c>
       <c r="H8">
-        <v>118</v>
+        <v>344</v>
       </c>
       <c r="I8">
-        <v>313</v>
+        <v>808</v>
       </c>
       <c r="J8">
-        <v>289</v>
+        <v>532</v>
       </c>
       <c r="K8">
-        <v>767</v>
+        <v>725</v>
       </c>
       <c r="L8">
-        <v>602</v>
+        <v>721</v>
       </c>
       <c r="M8">
-        <v>165</v>
+        <v>843</v>
       </c>
       <c r="N8">
-        <v>612</v>
+        <v>324</v>
       </c>
       <c r="O8">
-        <v>666</v>
+        <v>1</v>
       </c>
       <c r="P8">
-        <v>707</v>
+        <v>48</v>
       </c>
       <c r="Q8">
-        <v>891</v>
+        <v>339</v>
       </c>
       <c r="R8">
-        <v>337</v>
+        <v>457</v>
       </c>
       <c r="S8">
-        <v>73</v>
+        <v>172</v>
       </c>
       <c r="T8">
-        <v>836</v>
+        <v>772</v>
       </c>
       <c r="U8">
-        <v>140</v>
+        <v>625</v>
       </c>
       <c r="V8">
-        <v>160</v>
+        <v>589</v>
       </c>
       <c r="W8">
-        <v>261</v>
+        <v>846</v>
       </c>
       <c r="X8">
-        <v>598</v>
+        <v>865</v>
       </c>
       <c r="Y8">
-        <v>841</v>
+        <v>144</v>
       </c>
       <c r="Z8">
-        <v>183</v>
+        <v>209</v>
       </c>
       <c r="AA8">
-        <v>76</v>
+        <v>131</v>
       </c>
       <c r="AB8">
-        <v>808</v>
+        <v>24</v>
       </c>
       <c r="AC8">
-        <v>407</v>
+        <v>419</v>
       </c>
       <c r="AD8">
-        <v>742</v>
+        <v>815</v>
       </c>
       <c r="AE8">
-        <v>253</v>
+        <v>787</v>
       </c>
       <c r="AF8">
         <f t="shared" si="0"/>
@@ -1584,94 +1585,94 @@
     </row>
     <row r="9" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B9">
-        <v>335</v>
+        <v>398</v>
       </c>
       <c r="C9">
-        <v>122</v>
+        <v>22</v>
       </c>
       <c r="D9">
-        <v>781</v>
+        <v>876</v>
       </c>
       <c r="E9">
-        <v>798</v>
+        <v>555</v>
       </c>
       <c r="F9">
-        <v>635</v>
+        <v>401</v>
       </c>
       <c r="G9">
-        <v>322</v>
+        <v>425</v>
       </c>
       <c r="H9">
-        <v>433</v>
+        <v>76</v>
       </c>
       <c r="I9">
-        <v>775</v>
+        <v>757</v>
       </c>
       <c r="J9">
-        <v>740</v>
+        <v>531</v>
       </c>
       <c r="K9">
-        <v>706</v>
+        <v>128</v>
       </c>
       <c r="L9">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="M9">
-        <v>721</v>
+        <v>736</v>
       </c>
       <c r="N9">
-        <v>176</v>
+        <v>414</v>
       </c>
       <c r="O9">
-        <v>103</v>
+        <v>684</v>
       </c>
       <c r="P9">
-        <v>293</v>
+        <v>877</v>
       </c>
       <c r="Q9">
-        <v>672</v>
+        <v>688</v>
       </c>
       <c r="R9">
-        <v>787</v>
+        <v>329</v>
       </c>
       <c r="S9">
-        <v>109</v>
+        <v>803</v>
       </c>
       <c r="T9">
-        <v>287</v>
+        <v>655</v>
       </c>
       <c r="U9">
-        <v>668</v>
+        <v>424</v>
       </c>
       <c r="V9">
-        <v>382</v>
+        <v>824</v>
       </c>
       <c r="W9">
-        <v>478</v>
+        <v>553</v>
       </c>
       <c r="X9">
-        <v>213</v>
+        <v>7</v>
       </c>
       <c r="Y9">
-        <v>425</v>
+        <v>790</v>
       </c>
       <c r="Z9">
-        <v>406</v>
+        <v>27</v>
       </c>
       <c r="AA9">
-        <v>245</v>
+        <v>92</v>
       </c>
       <c r="AB9">
-        <v>870</v>
+        <v>186</v>
       </c>
       <c r="AC9">
-        <v>341</v>
+        <v>697</v>
       </c>
       <c r="AD9">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="AE9">
-        <v>528</v>
+        <v>442</v>
       </c>
       <c r="AF9">
         <f t="shared" si="0"/>
@@ -1680,94 +1681,94 @@
     </row>
     <row r="10" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B10">
-        <v>458</v>
+        <v>418</v>
       </c>
       <c r="C10">
-        <v>810</v>
+        <v>656</v>
       </c>
       <c r="D10">
-        <v>695</v>
+        <v>196</v>
       </c>
       <c r="E10">
-        <v>751</v>
+        <v>472</v>
       </c>
       <c r="F10">
-        <v>420</v>
+        <v>714</v>
       </c>
       <c r="G10">
-        <v>768</v>
+        <v>444</v>
       </c>
       <c r="H10">
-        <v>655</v>
+        <v>528</v>
       </c>
       <c r="I10">
-        <v>85</v>
+        <v>633</v>
       </c>
       <c r="J10">
-        <v>605</v>
+        <v>512</v>
       </c>
       <c r="K10">
-        <v>678</v>
+        <v>896</v>
       </c>
       <c r="L10">
-        <v>673</v>
+        <v>435</v>
       </c>
       <c r="M10">
-        <v>770</v>
+        <v>201</v>
       </c>
       <c r="N10">
-        <v>507</v>
+        <v>49</v>
       </c>
       <c r="O10">
-        <v>456</v>
+        <v>294</v>
       </c>
       <c r="P10">
-        <v>536</v>
+        <v>110</v>
       </c>
       <c r="Q10">
-        <v>53</v>
+        <v>509</v>
       </c>
       <c r="R10">
-        <v>25</v>
+        <v>268</v>
       </c>
       <c r="S10">
-        <v>469</v>
+        <v>651</v>
       </c>
       <c r="T10">
-        <v>443</v>
+        <v>819</v>
       </c>
       <c r="U10">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="V10">
-        <v>317</v>
+        <v>595</v>
       </c>
       <c r="W10">
-        <v>278</v>
+        <v>554</v>
       </c>
       <c r="X10">
-        <v>3</v>
+        <v>275</v>
       </c>
       <c r="Y10">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="Z10">
-        <v>58</v>
+        <v>222</v>
       </c>
       <c r="AA10">
-        <v>615</v>
+        <v>461</v>
       </c>
       <c r="AB10">
-        <v>480</v>
+        <v>234</v>
       </c>
       <c r="AC10">
-        <v>716</v>
+        <v>483</v>
       </c>
       <c r="AD10">
-        <v>395</v>
+        <v>861</v>
       </c>
       <c r="AE10">
-        <v>380</v>
+        <v>643</v>
       </c>
       <c r="AF10">
         <f t="shared" si="0"/>
@@ -1776,94 +1777,94 @@
     </row>
     <row r="11" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B11">
-        <v>132</v>
+        <v>439</v>
       </c>
       <c r="C11">
-        <v>40</v>
+        <v>174</v>
       </c>
       <c r="D11">
-        <v>78</v>
+        <v>376</v>
       </c>
       <c r="E11">
-        <v>93</v>
+        <v>663</v>
       </c>
       <c r="F11">
-        <v>291</v>
+        <v>382</v>
       </c>
       <c r="G11">
-        <v>557</v>
+        <v>602</v>
       </c>
       <c r="H11">
-        <v>124</v>
+        <v>879</v>
       </c>
       <c r="I11">
-        <v>470</v>
+        <v>214</v>
       </c>
       <c r="J11">
-        <v>254</v>
+        <v>311</v>
       </c>
       <c r="K11">
-        <v>596</v>
+        <v>216</v>
       </c>
       <c r="L11">
+        <v>648</v>
+      </c>
+      <c r="M11">
+        <v>713</v>
+      </c>
+      <c r="N11">
+        <v>41</v>
+      </c>
+      <c r="O11">
+        <v>854</v>
+      </c>
+      <c r="P11">
+        <v>712</v>
+      </c>
+      <c r="Q11">
+        <v>356</v>
+      </c>
+      <c r="R11">
+        <v>493</v>
+      </c>
+      <c r="S11">
+        <v>307</v>
+      </c>
+      <c r="T11">
+        <v>50</v>
+      </c>
+      <c r="U11">
+        <v>759</v>
+      </c>
+      <c r="V11">
+        <v>400</v>
+      </c>
+      <c r="W11">
+        <v>227</v>
+      </c>
+      <c r="X11">
+        <v>253</v>
+      </c>
+      <c r="Y11">
+        <v>481</v>
+      </c>
+      <c r="Z11">
         <v>709</v>
       </c>
-      <c r="M11">
-        <v>843</v>
-      </c>
-      <c r="N11">
-        <v>873</v>
-      </c>
-      <c r="O11">
-        <v>683</v>
-      </c>
-      <c r="P11">
-        <v>207</v>
-      </c>
-      <c r="Q11">
-        <v>191</v>
-      </c>
-      <c r="R11">
-        <v>534</v>
-      </c>
-      <c r="S11">
-        <v>285</v>
-      </c>
-      <c r="T11">
-        <v>619</v>
-      </c>
-      <c r="U11">
-        <v>457</v>
-      </c>
-      <c r="V11">
-        <v>827</v>
-      </c>
-      <c r="W11">
-        <v>68</v>
-      </c>
-      <c r="X11">
-        <v>670</v>
-      </c>
-      <c r="Y11">
-        <v>486</v>
-      </c>
-      <c r="Z11">
-        <v>654</v>
-      </c>
       <c r="AA11">
-        <v>589</v>
+        <v>403</v>
       </c>
       <c r="AB11">
-        <v>131</v>
+        <v>586</v>
       </c>
       <c r="AC11">
-        <v>835</v>
+        <v>840</v>
       </c>
       <c r="AD11">
-        <v>332</v>
+        <v>167</v>
       </c>
       <c r="AE11">
-        <v>887</v>
+        <v>260</v>
       </c>
       <c r="AF11">
         <f t="shared" si="0"/>
@@ -1872,94 +1873,94 @@
     </row>
     <row r="12" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B12">
-        <v>715</v>
+        <v>247</v>
       </c>
       <c r="C12">
-        <v>168</v>
+        <v>850</v>
       </c>
       <c r="D12">
-        <v>260</v>
+        <v>296</v>
       </c>
       <c r="E12">
-        <v>640</v>
+        <v>809</v>
       </c>
       <c r="F12">
-        <v>821</v>
+        <v>724</v>
       </c>
       <c r="G12">
-        <v>249</v>
+        <v>789</v>
       </c>
       <c r="H12">
-        <v>701</v>
+        <v>726</v>
       </c>
       <c r="I12">
-        <v>696</v>
+        <v>26</v>
       </c>
       <c r="J12">
-        <v>515</v>
+        <v>175</v>
       </c>
       <c r="K12">
-        <v>756</v>
+        <v>762</v>
       </c>
       <c r="L12">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="M12">
-        <v>27</v>
+        <v>124</v>
       </c>
       <c r="N12">
-        <v>900</v>
+        <v>65</v>
       </c>
       <c r="O12">
-        <v>599</v>
+        <v>800</v>
       </c>
       <c r="P12">
-        <v>147</v>
+        <v>514</v>
       </c>
       <c r="Q12">
-        <v>208</v>
+        <v>662</v>
       </c>
       <c r="R12">
-        <v>22</v>
+        <v>402</v>
       </c>
       <c r="S12">
-        <v>112</v>
+        <v>541</v>
       </c>
       <c r="T12">
-        <v>546</v>
+        <v>706</v>
       </c>
       <c r="U12">
+        <v>53</v>
+      </c>
+      <c r="V12">
+        <v>466</v>
+      </c>
+      <c r="W12">
+        <v>475</v>
+      </c>
+      <c r="X12">
+        <v>527</v>
+      </c>
+      <c r="Y12">
+        <v>573</v>
+      </c>
+      <c r="Z12">
+        <v>596</v>
+      </c>
+      <c r="AA12">
         <v>367</v>
       </c>
-      <c r="V12">
-        <v>622</v>
-      </c>
-      <c r="W12">
-        <v>860</v>
-      </c>
-      <c r="X12">
-        <v>744</v>
-      </c>
-      <c r="Y12">
-        <v>65</v>
-      </c>
-      <c r="Z12">
-        <v>845</v>
-      </c>
-      <c r="AA12">
-        <v>9</v>
-      </c>
       <c r="AB12">
-        <v>535</v>
+        <v>30</v>
       </c>
       <c r="AC12">
-        <v>298</v>
+        <v>28</v>
       </c>
       <c r="AD12">
-        <v>269</v>
+        <v>237</v>
       </c>
       <c r="AE12">
-        <v>352</v>
+        <v>494</v>
       </c>
       <c r="AF12">
         <f t="shared" si="0"/>
@@ -1968,94 +1969,94 @@
     </row>
     <row r="13" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B13">
-        <v>259</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>219</v>
+        <v>636</v>
       </c>
       <c r="D13">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="E13">
-        <v>182</v>
+        <v>867</v>
       </c>
       <c r="F13">
-        <v>790</v>
+        <v>812</v>
       </c>
       <c r="G13">
-        <v>404</v>
+        <v>199</v>
       </c>
       <c r="H13">
-        <v>849</v>
+        <v>722</v>
       </c>
       <c r="I13">
-        <v>691</v>
+        <v>240</v>
       </c>
       <c r="J13">
-        <v>206</v>
+        <v>848</v>
       </c>
       <c r="K13">
-        <v>807</v>
+        <v>432</v>
       </c>
       <c r="L13">
-        <v>174</v>
+        <v>607</v>
       </c>
       <c r="M13">
-        <v>703</v>
+        <v>627</v>
       </c>
       <c r="N13">
-        <v>96</v>
+        <v>169</v>
       </c>
       <c r="O13">
-        <v>70</v>
+        <v>834</v>
       </c>
       <c r="P13">
-        <v>595</v>
+        <v>501</v>
       </c>
       <c r="Q13">
-        <v>573</v>
+        <v>20</v>
       </c>
       <c r="R13">
-        <v>760</v>
+        <v>670</v>
       </c>
       <c r="S13">
-        <v>511</v>
+        <v>417</v>
       </c>
       <c r="T13">
-        <v>47</v>
+        <v>548</v>
       </c>
       <c r="U13">
-        <v>880</v>
+        <v>391</v>
       </c>
       <c r="V13">
-        <v>414</v>
+        <v>360</v>
       </c>
       <c r="W13">
-        <v>426</v>
+        <v>383</v>
       </c>
       <c r="X13">
-        <v>567</v>
+        <v>154</v>
       </c>
       <c r="Y13">
-        <v>765</v>
+        <v>479</v>
       </c>
       <c r="Z13">
-        <v>61</v>
+        <v>546</v>
       </c>
       <c r="AA13">
-        <v>699</v>
+        <v>802</v>
       </c>
       <c r="AB13">
-        <v>391</v>
+        <v>539</v>
       </c>
       <c r="AC13">
-        <v>579</v>
+        <v>283</v>
       </c>
       <c r="AD13">
-        <v>190</v>
+        <v>79</v>
       </c>
       <c r="AE13">
-        <v>576</v>
+        <v>207</v>
       </c>
       <c r="AF13">
         <f t="shared" si="0"/>
@@ -2064,94 +2065,94 @@
     </row>
     <row r="14" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B14">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C14">
-        <v>591</v>
+        <v>797</v>
       </c>
       <c r="D14">
-        <v>504</v>
+        <v>181</v>
       </c>
       <c r="E14">
-        <v>753</v>
+        <v>487</v>
       </c>
       <c r="F14">
-        <v>166</v>
+        <v>143</v>
       </c>
       <c r="G14">
-        <v>34</v>
+        <v>561</v>
       </c>
       <c r="H14">
-        <v>383</v>
+        <v>452</v>
       </c>
       <c r="I14">
-        <v>343</v>
+        <v>818</v>
       </c>
       <c r="J14">
-        <v>801</v>
+        <v>773</v>
       </c>
       <c r="K14">
-        <v>475</v>
+        <v>78</v>
       </c>
       <c r="L14">
-        <v>163</v>
+        <v>218</v>
       </c>
       <c r="M14">
-        <v>686</v>
+        <v>664</v>
       </c>
       <c r="N14">
-        <v>86</v>
+        <v>614</v>
       </c>
       <c r="O14">
-        <v>523</v>
+        <v>871</v>
       </c>
       <c r="P14">
-        <v>747</v>
+        <v>64</v>
       </c>
       <c r="Q14">
-        <v>885</v>
+        <v>710</v>
       </c>
       <c r="R14">
-        <v>474</v>
+        <v>117</v>
       </c>
       <c r="S14">
-        <v>459</v>
+        <v>146</v>
       </c>
       <c r="T14">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="U14">
-        <v>150</v>
+        <v>82</v>
       </c>
       <c r="V14">
-        <v>386</v>
+        <v>560</v>
       </c>
       <c r="W14">
-        <v>687</v>
+        <v>242</v>
       </c>
       <c r="X14">
-        <v>609</v>
+        <v>254</v>
       </c>
       <c r="Y14">
-        <v>840</v>
+        <v>545</v>
       </c>
       <c r="Z14">
-        <v>782</v>
+        <v>700</v>
       </c>
       <c r="AA14">
-        <v>859</v>
+        <v>680</v>
       </c>
       <c r="AB14">
-        <v>51</v>
+        <v>767</v>
       </c>
       <c r="AC14">
-        <v>196</v>
+        <v>779</v>
       </c>
       <c r="AD14">
-        <v>144</v>
+        <v>658</v>
       </c>
       <c r="AE14">
-        <v>442</v>
+        <v>180</v>
       </c>
       <c r="AF14">
         <f t="shared" si="0"/>
@@ -2160,94 +2161,94 @@
     </row>
     <row r="15" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B15">
+        <v>235</v>
+      </c>
+      <c r="C15">
         <v>571</v>
       </c>
-      <c r="C15">
-        <v>623</v>
-      </c>
       <c r="D15">
-        <v>446</v>
+        <v>628</v>
       </c>
       <c r="E15">
-        <v>600</v>
+        <v>829</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>875</v>
       </c>
       <c r="G15">
-        <v>388</v>
+        <v>52</v>
       </c>
       <c r="H15">
-        <v>680</v>
+        <v>632</v>
       </c>
       <c r="I15">
-        <v>333</v>
+        <v>100</v>
       </c>
       <c r="J15">
-        <v>639</v>
+        <v>220</v>
       </c>
       <c r="K15">
-        <v>464</v>
+        <v>342</v>
       </c>
       <c r="L15">
-        <v>444</v>
+        <v>582</v>
       </c>
       <c r="M15">
-        <v>49</v>
+        <v>105</v>
       </c>
       <c r="N15">
-        <v>115</v>
+        <v>538</v>
       </c>
       <c r="O15">
-        <v>553</v>
+        <v>219</v>
       </c>
       <c r="P15">
-        <v>608</v>
+        <v>526</v>
       </c>
       <c r="Q15">
-        <v>327</v>
+        <v>372</v>
       </c>
       <c r="R15">
-        <v>714</v>
+        <v>677</v>
       </c>
       <c r="S15">
-        <v>501</v>
+        <v>810</v>
       </c>
       <c r="T15">
-        <v>325</v>
+        <v>226</v>
       </c>
       <c r="U15">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="V15">
-        <v>651</v>
+        <v>671</v>
       </c>
       <c r="W15">
-        <v>424</v>
+        <v>250</v>
       </c>
       <c r="X15">
-        <v>830</v>
+        <v>189</v>
       </c>
       <c r="Y15">
-        <v>855</v>
+        <v>659</v>
       </c>
       <c r="Z15">
-        <v>308</v>
+        <v>139</v>
       </c>
       <c r="AA15">
-        <v>389</v>
+        <v>489</v>
       </c>
       <c r="AB15">
-        <v>212</v>
+        <v>675</v>
       </c>
       <c r="AC15">
-        <v>173</v>
+        <v>774</v>
       </c>
       <c r="AD15">
-        <v>723</v>
+        <v>707</v>
       </c>
       <c r="AE15">
-        <v>532</v>
+        <v>352</v>
       </c>
       <c r="AF15">
         <f t="shared" si="0"/>
@@ -2256,94 +2257,94 @@
     </row>
     <row r="16" spans="2:32" x14ac:dyDescent="0.2">
       <c r="B16">
-        <v>516</v>
+        <v>224</v>
       </c>
       <c r="C16">
-        <v>263</v>
+        <v>305</v>
       </c>
       <c r="D16">
-        <v>365</v>
+        <v>265</v>
       </c>
       <c r="E16">
-        <v>412</v>
+        <v>232</v>
       </c>
       <c r="F16">
-        <v>288</v>
+        <v>883</v>
       </c>
       <c r="G16">
-        <v>79</v>
+        <v>446</v>
       </c>
       <c r="H16">
-        <v>403</v>
+        <v>51</v>
       </c>
       <c r="I16">
-        <v>418</v>
+        <v>81</v>
       </c>
       <c r="J16">
-        <v>421</v>
+        <v>763</v>
       </c>
       <c r="K16">
-        <v>14</v>
+        <v>413</v>
       </c>
       <c r="L16">
-        <v>587</v>
+        <v>431</v>
       </c>
       <c r="M16">
-        <v>347</v>
+        <v>173</v>
       </c>
       <c r="N16">
-        <v>627</v>
+        <v>780</v>
       </c>
       <c r="O16">
-        <v>624</v>
+        <v>423</v>
       </c>
       <c r="P16">
-        <v>818</v>
+        <v>653</v>
       </c>
       <c r="Q16">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="R16">
-        <v>824</v>
+        <v>17</v>
       </c>
       <c r="S16">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="T16">
-        <v>256</v>
+        <v>111</v>
       </c>
       <c r="U16">
-        <v>417</v>
+        <v>756</v>
       </c>
       <c r="V16">
-        <v>737</v>
+        <v>716</v>
       </c>
       <c r="W16">
-        <v>811</v>
+        <v>145</v>
       </c>
       <c r="X16">
-        <v>346</v>
+        <v>639</v>
       </c>
       <c r="Y16">
-        <v>492</v>
+        <v>777</v>
       </c>
       <c r="Z16">
-        <v>713</v>
+        <v>768</v>
       </c>
       <c r="AA16">
-        <v>280</v>
+        <v>657</v>
       </c>
       <c r="AB16">
-        <v>488</v>
+        <v>84</v>
       </c>
       <c r="AC16">
-        <v>217</v>
+        <v>101</v>
       </c>
       <c r="AD16">
-        <v>137</v>
+        <v>629</v>
       </c>
       <c r="AE16">
-        <v>189</v>
+        <v>566</v>
       </c>
       <c r="AF16">
         <f t="shared" si="0"/>
@@ -2352,94 +2353,94 @@
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B17">
-        <v>149</v>
+        <v>740</v>
       </c>
       <c r="C17">
-        <v>570</v>
+        <v>591</v>
       </c>
       <c r="D17">
-        <v>871</v>
+        <v>164</v>
       </c>
       <c r="E17">
-        <v>251</v>
+        <v>515</v>
       </c>
       <c r="F17">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="G17">
-        <v>564</v>
+        <v>447</v>
       </c>
       <c r="H17">
-        <v>566</v>
+        <v>407</v>
       </c>
       <c r="I17">
-        <v>234</v>
+        <v>468</v>
       </c>
       <c r="J17">
-        <v>5</v>
+        <v>297</v>
       </c>
       <c r="K17">
-        <v>882</v>
+        <v>511</v>
       </c>
       <c r="L17">
-        <v>468</v>
+        <v>743</v>
       </c>
       <c r="M17">
-        <v>894</v>
+        <v>618</v>
       </c>
       <c r="N17">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="O17">
-        <v>594</v>
+        <v>437</v>
       </c>
       <c r="P17">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="Q17">
-        <v>411</v>
+        <v>252</v>
       </c>
       <c r="R17">
-        <v>334</v>
+        <v>29</v>
       </c>
       <c r="S17">
-        <v>218</v>
+        <v>682</v>
       </c>
       <c r="T17">
-        <v>436</v>
+        <v>838</v>
       </c>
       <c r="U17">
-        <v>445</v>
+        <v>161</v>
       </c>
       <c r="V17">
-        <v>890</v>
+        <v>249</v>
       </c>
       <c r="W17">
-        <v>387</v>
+        <v>399</v>
       </c>
       <c r="X17">
-        <v>650</v>
+        <v>827</v>
       </c>
       <c r="Y17">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="Z17">
-        <v>321</v>
+        <v>162</v>
       </c>
       <c r="AA17">
-        <v>440</v>
+        <v>404</v>
       </c>
       <c r="AB17">
-        <v>104</v>
+        <v>753</v>
       </c>
       <c r="AC17">
-        <v>846</v>
+        <v>839</v>
       </c>
       <c r="AD17">
-        <v>295</v>
+        <v>152</v>
       </c>
       <c r="AE17">
-        <v>498</v>
+        <v>691</v>
       </c>
       <c r="AF17">
         <f t="shared" si="0"/>
@@ -2448,94 +2449,94 @@
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B18">
-        <v>592</v>
+        <v>97</v>
       </c>
       <c r="C18">
-        <v>588</v>
+        <v>31</v>
       </c>
       <c r="D18">
-        <v>484</v>
+        <v>552</v>
       </c>
       <c r="E18">
-        <v>662</v>
+        <v>39</v>
       </c>
       <c r="F18">
-        <v>164</v>
+        <v>581</v>
       </c>
       <c r="G18">
-        <v>363</v>
+        <v>192</v>
       </c>
       <c r="H18">
-        <v>494</v>
+        <v>261</v>
       </c>
       <c r="I18">
-        <v>856</v>
+        <v>775</v>
       </c>
       <c r="J18">
-        <v>186</v>
+        <v>737</v>
       </c>
       <c r="K18">
-        <v>463</v>
+        <v>338</v>
       </c>
       <c r="L18">
-        <v>530</v>
+        <v>364</v>
       </c>
       <c r="M18">
-        <v>375</v>
+        <v>499</v>
       </c>
       <c r="N18">
-        <v>108</v>
+        <v>719</v>
       </c>
       <c r="O18">
-        <v>180</v>
+        <v>882</v>
       </c>
       <c r="P18">
-        <v>577</v>
+        <v>55</v>
       </c>
       <c r="Q18">
-        <v>634</v>
+        <v>326</v>
       </c>
       <c r="R18">
-        <v>820</v>
+        <v>782</v>
       </c>
       <c r="S18">
-        <v>777</v>
+        <v>426</v>
       </c>
       <c r="T18">
-        <v>290</v>
+        <v>448</v>
       </c>
       <c r="U18">
-        <v>607</v>
+        <v>758</v>
       </c>
       <c r="V18">
-        <v>223</v>
+        <v>519</v>
       </c>
       <c r="W18">
-        <v>2</v>
+        <v>534</v>
       </c>
       <c r="X18">
-        <v>339</v>
+        <v>769</v>
       </c>
       <c r="Y18">
-        <v>71</v>
+        <v>370</v>
       </c>
       <c r="Z18">
-        <v>561</v>
+        <v>102</v>
       </c>
       <c r="AA18">
-        <v>551</v>
+        <v>486</v>
       </c>
       <c r="AB18">
-        <v>838</v>
+        <v>686</v>
       </c>
       <c r="AC18">
-        <v>255</v>
+        <v>113</v>
       </c>
       <c r="AD18">
-        <v>804</v>
+        <v>823</v>
       </c>
       <c r="AE18">
-        <v>121</v>
+        <v>251</v>
       </c>
       <c r="AF18">
         <f t="shared" si="0"/>
@@ -2544,94 +2545,94 @@
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B19">
+        <v>523</v>
+      </c>
+      <c r="C19">
+        <v>351</v>
+      </c>
+      <c r="D19">
+        <v>208</v>
+      </c>
+      <c r="E19">
+        <v>711</v>
+      </c>
+      <c r="F19">
+        <v>333</v>
+      </c>
+      <c r="G19">
+        <v>567</v>
+      </c>
+      <c r="H19">
+        <v>695</v>
+      </c>
+      <c r="I19">
+        <v>366</v>
+      </c>
+      <c r="J19">
+        <v>530</v>
+      </c>
+      <c r="K19">
+        <v>441</v>
+      </c>
+      <c r="L19">
+        <v>422</v>
+      </c>
+      <c r="M19">
+        <v>488</v>
+      </c>
+      <c r="N19">
+        <v>380</v>
+      </c>
+      <c r="O19">
+        <v>257</v>
+      </c>
+      <c r="P19">
+        <v>359</v>
+      </c>
+      <c r="Q19">
+        <v>286</v>
+      </c>
+      <c r="R19">
+        <v>299</v>
+      </c>
+      <c r="S19">
+        <v>182</v>
+      </c>
+      <c r="T19">
+        <v>3</v>
+      </c>
+      <c r="U19">
+        <v>747</v>
+      </c>
+      <c r="V19">
+        <v>302</v>
+      </c>
+      <c r="W19">
+        <v>752</v>
+      </c>
+      <c r="X19">
+        <v>279</v>
+      </c>
+      <c r="Y19">
+        <v>156</v>
+      </c>
+      <c r="Z19">
+        <v>785</v>
+      </c>
+      <c r="AA19">
+        <v>308</v>
+      </c>
+      <c r="AB19">
+        <v>836</v>
+      </c>
+      <c r="AC19">
+        <v>728</v>
+      </c>
+      <c r="AD19">
         <v>455</v>
       </c>
-      <c r="C19">
-        <v>733</v>
-      </c>
-      <c r="D19">
-        <v>188</v>
-      </c>
-      <c r="E19">
-        <v>712</v>
-      </c>
-      <c r="F19">
-        <v>377</v>
-      </c>
-      <c r="G19">
-        <v>390</v>
-      </c>
-      <c r="H19">
-        <v>731</v>
-      </c>
-      <c r="I19">
-        <v>146</v>
-      </c>
-      <c r="J19">
-        <v>162</v>
-      </c>
-      <c r="K19">
-        <v>739</v>
-      </c>
-      <c r="L19">
-        <v>743</v>
-      </c>
-      <c r="M19">
-        <v>46</v>
-      </c>
-      <c r="N19">
-        <v>490</v>
-      </c>
-      <c r="O19">
-        <v>210</v>
-      </c>
-      <c r="P19">
-        <v>637</v>
-      </c>
-      <c r="Q19">
-        <v>355</v>
-      </c>
-      <c r="R19">
-        <v>537</v>
-      </c>
-      <c r="S19">
-        <v>309</v>
-      </c>
-      <c r="T19">
-        <v>684</v>
-      </c>
-      <c r="U19">
-        <v>669</v>
-      </c>
-      <c r="V19">
-        <v>698</v>
-      </c>
-      <c r="W19">
-        <v>617</v>
-      </c>
-      <c r="X19">
-        <v>184</v>
-      </c>
-      <c r="Y19">
-        <v>231</v>
-      </c>
-      <c r="Z19">
-        <v>300</v>
-      </c>
-      <c r="AA19">
-        <v>94</v>
-      </c>
-      <c r="AB19">
-        <v>784</v>
-      </c>
-      <c r="AC19">
-        <v>632</v>
-      </c>
-      <c r="AD19">
-        <v>292</v>
-      </c>
       <c r="AE19">
-        <v>370</v>
+        <v>766</v>
       </c>
       <c r="AF19">
         <f t="shared" si="0"/>
@@ -2640,94 +2641,94 @@
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B20">
-        <v>461</v>
+        <v>609</v>
       </c>
       <c r="C20">
-        <v>267</v>
+        <v>119</v>
       </c>
       <c r="D20">
-        <v>806</v>
+        <v>889</v>
       </c>
       <c r="E20">
-        <v>111</v>
+        <v>490</v>
       </c>
       <c r="F20">
-        <v>729</v>
+        <v>108</v>
       </c>
       <c r="G20">
-        <v>271</v>
+        <v>115</v>
       </c>
       <c r="H20">
-        <v>329</v>
+        <v>869</v>
       </c>
       <c r="I20">
-        <v>529</v>
+        <v>330</v>
       </c>
       <c r="J20">
-        <v>653</v>
+        <v>584</v>
       </c>
       <c r="K20">
-        <v>362</v>
+        <v>415</v>
       </c>
       <c r="L20">
-        <v>294</v>
+        <v>694</v>
       </c>
       <c r="M20">
-        <v>788</v>
+        <v>59</v>
       </c>
       <c r="N20">
-        <v>326</v>
+        <v>480</v>
       </c>
       <c r="O20">
-        <v>481</v>
+        <v>295</v>
       </c>
       <c r="P20">
-        <v>659</v>
+        <v>612</v>
       </c>
       <c r="Q20">
-        <v>558</v>
+        <v>378</v>
       </c>
       <c r="R20">
-        <v>17</v>
+        <v>623</v>
       </c>
       <c r="S20">
-        <v>413</v>
+        <v>322</v>
       </c>
       <c r="T20">
-        <v>861</v>
+        <v>590</v>
       </c>
       <c r="U20">
-        <v>688</v>
+        <v>138</v>
       </c>
       <c r="V20">
-        <v>419</v>
+        <v>547</v>
       </c>
       <c r="W20">
-        <v>139</v>
+        <v>749</v>
       </c>
       <c r="X20">
-        <v>525</v>
+        <v>13</v>
       </c>
       <c r="Y20">
-        <v>204</v>
+        <v>91</v>
       </c>
       <c r="Z20">
-        <v>209</v>
+        <v>674</v>
       </c>
       <c r="AA20">
-        <v>286</v>
+        <v>318</v>
       </c>
       <c r="AB20">
-        <v>748</v>
+        <v>770</v>
       </c>
       <c r="AC20">
-        <v>460</v>
+        <v>474</v>
       </c>
       <c r="AD20">
-        <v>500</v>
+        <v>886</v>
       </c>
       <c r="AE20">
-        <v>422</v>
+        <v>274</v>
       </c>
       <c r="AF20">
         <f t="shared" si="0"/>
@@ -2736,94 +2737,94 @@
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B21">
-        <v>20</v>
+        <v>895</v>
       </c>
       <c r="C21">
-        <v>483</v>
+        <v>300</v>
       </c>
       <c r="D21">
-        <v>379</v>
+        <v>406</v>
       </c>
       <c r="E21">
-        <v>512</v>
+        <v>563</v>
       </c>
       <c r="F21">
-        <v>735</v>
+        <v>94</v>
       </c>
       <c r="G21">
-        <v>211</v>
+        <v>454</v>
       </c>
       <c r="H21">
-        <v>508</v>
+        <v>851</v>
       </c>
       <c r="I21">
-        <v>281</v>
+        <v>349</v>
       </c>
       <c r="J21">
-        <v>170</v>
+        <v>357</v>
       </c>
       <c r="K21">
-        <v>482</v>
+        <v>557</v>
       </c>
       <c r="L21">
-        <v>829</v>
+        <v>270</v>
       </c>
       <c r="M21">
-        <v>270</v>
+        <v>529</v>
       </c>
       <c r="N21">
-        <v>693</v>
+        <v>58</v>
       </c>
       <c r="O21">
-        <v>556</v>
+        <v>358</v>
       </c>
       <c r="P21">
-        <v>318</v>
+        <v>450</v>
       </c>
       <c r="Q21">
-        <v>867</v>
+        <v>822</v>
       </c>
       <c r="R21">
-        <v>584</v>
+        <v>312</v>
       </c>
       <c r="S21">
-        <v>138</v>
+        <v>703</v>
       </c>
       <c r="T21">
-        <v>44</v>
+        <v>277</v>
       </c>
       <c r="U21">
-        <v>834</v>
+        <v>568</v>
       </c>
       <c r="V21">
-        <v>519</v>
+        <v>579</v>
       </c>
       <c r="W21">
-        <v>506</v>
+        <v>626</v>
       </c>
       <c r="X21">
-        <v>328</v>
+        <v>660</v>
       </c>
       <c r="Y21">
-        <v>495</v>
+        <v>36</v>
       </c>
       <c r="Z21">
-        <v>652</v>
+        <v>537</v>
       </c>
       <c r="AA21">
-        <v>874</v>
+        <v>134</v>
       </c>
       <c r="AB21">
-        <v>89</v>
+        <v>599</v>
       </c>
       <c r="AC21">
-        <v>257</v>
+        <v>93</v>
       </c>
       <c r="AD21">
-        <v>776</v>
+        <v>642</v>
       </c>
       <c r="AE21">
-        <v>105</v>
+        <v>436</v>
       </c>
       <c r="AF21">
         <f t="shared" si="0"/>
@@ -2832,94 +2833,94 @@
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B22">
-        <v>658</v>
+        <v>892</v>
       </c>
       <c r="C22">
-        <v>305</v>
+        <v>781</v>
       </c>
       <c r="D22">
-        <v>143</v>
+        <v>606</v>
       </c>
       <c r="E22">
-        <v>185</v>
+        <v>166</v>
       </c>
       <c r="F22">
-        <v>745</v>
+        <v>482</v>
       </c>
       <c r="G22">
-        <v>524</v>
+        <v>619</v>
       </c>
       <c r="H22">
-        <v>142</v>
+        <v>200</v>
       </c>
       <c r="I22">
-        <v>889</v>
+        <v>536</v>
       </c>
       <c r="J22">
-        <v>116</v>
+        <v>225</v>
       </c>
       <c r="K22">
-        <v>819</v>
+        <v>18</v>
       </c>
       <c r="L22">
-        <v>423</v>
+        <v>377</v>
       </c>
       <c r="M22">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="N22">
-        <v>825</v>
+        <v>853</v>
       </c>
       <c r="O22">
-        <v>493</v>
+        <v>429</v>
       </c>
       <c r="P22">
-        <v>126</v>
+        <v>428</v>
       </c>
       <c r="Q22">
-        <v>349</v>
+        <v>574</v>
       </c>
       <c r="R22">
-        <v>235</v>
+        <v>592</v>
       </c>
       <c r="S22">
-        <v>521</v>
+        <v>485</v>
       </c>
       <c r="T22">
-        <v>633</v>
+        <v>179</v>
       </c>
       <c r="U22">
-        <v>167</v>
+        <v>361</v>
       </c>
       <c r="V22">
-        <v>826</v>
+        <v>88</v>
       </c>
       <c r="W22">
-        <v>348</v>
+        <v>171</v>
       </c>
       <c r="X22">
-        <v>601</v>
+        <v>652</v>
       </c>
       <c r="Y22">
-        <v>128</v>
+        <v>699</v>
       </c>
       <c r="Z22">
-        <v>786</v>
+        <v>761</v>
       </c>
       <c r="AA22">
-        <v>175</v>
+        <v>284</v>
       </c>
       <c r="AB22">
-        <v>758</v>
+        <v>303</v>
       </c>
       <c r="AC22">
-        <v>660</v>
+        <v>638</v>
       </c>
       <c r="AD22">
-        <v>505</v>
+        <v>835</v>
       </c>
       <c r="AE22">
-        <v>274</v>
+        <v>130</v>
       </c>
       <c r="AF22">
         <f t="shared" si="0"/>
@@ -2928,94 +2929,94 @@
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B23">
-        <v>773</v>
+        <v>85</v>
       </c>
       <c r="C23">
-        <v>324</v>
+        <v>375</v>
       </c>
       <c r="D23">
-        <v>311</v>
+        <v>731</v>
       </c>
       <c r="E23">
+        <v>354</v>
+      </c>
+      <c r="F23">
+        <v>715</v>
+      </c>
+      <c r="G23">
+        <v>855</v>
+      </c>
+      <c r="H23">
+        <v>70</v>
+      </c>
+      <c r="I23">
+        <v>828</v>
+      </c>
+      <c r="J23">
+        <v>616</v>
+      </c>
+      <c r="K23">
+        <v>66</v>
+      </c>
+      <c r="L23">
+        <v>98</v>
+      </c>
+      <c r="M23">
+        <v>852</v>
+      </c>
+      <c r="N23">
+        <v>771</v>
+      </c>
+      <c r="O23">
+        <v>223</v>
+      </c>
+      <c r="P23">
+        <v>624</v>
+      </c>
+      <c r="Q23">
+        <v>746</v>
+      </c>
+      <c r="R23">
+        <v>246</v>
+      </c>
+      <c r="S23">
+        <v>411</v>
+      </c>
+      <c r="T23">
+        <v>238</v>
+      </c>
+      <c r="U23">
+        <v>841</v>
+      </c>
+      <c r="V23">
+        <v>345</v>
+      </c>
+      <c r="W23">
+        <v>856</v>
+      </c>
+      <c r="X23">
+        <v>416</v>
+      </c>
+      <c r="Y23">
+        <v>60</v>
+      </c>
+      <c r="Z23">
+        <v>778</v>
+      </c>
+      <c r="AA23">
+        <v>325</v>
+      </c>
+      <c r="AB23">
+        <v>386</v>
+      </c>
+      <c r="AC23">
+        <v>558</v>
+      </c>
+      <c r="AD23">
+        <v>34</v>
+      </c>
+      <c r="AE23">
         <v>12</v>
-      </c>
-      <c r="F23">
-        <v>779</v>
-      </c>
-      <c r="G23">
-        <v>526</v>
-      </c>
-      <c r="H23">
-        <v>816</v>
-      </c>
-      <c r="I23">
-        <v>881</v>
-      </c>
-      <c r="J23">
-        <v>728</v>
-      </c>
-      <c r="K23">
-        <v>549</v>
-      </c>
-      <c r="L23">
-        <v>477</v>
-      </c>
-      <c r="M23">
-        <v>641</v>
-      </c>
-      <c r="N23">
-        <v>434</v>
-      </c>
-      <c r="O23">
-        <v>893</v>
-      </c>
-      <c r="P23">
-        <v>629</v>
-      </c>
-      <c r="Q23">
-        <v>30</v>
-      </c>
-      <c r="R23">
-        <v>439</v>
-      </c>
-      <c r="S23">
-        <v>90</v>
-      </c>
-      <c r="T23">
-        <v>554</v>
-      </c>
-      <c r="U23">
-        <v>228</v>
-      </c>
-      <c r="V23">
-        <v>88</v>
-      </c>
-      <c r="W23">
-        <v>771</v>
-      </c>
-      <c r="X23">
-        <v>307</v>
-      </c>
-      <c r="Y23">
-        <v>822</v>
-      </c>
-      <c r="Z23">
-        <v>38</v>
-      </c>
-      <c r="AA23">
-        <v>145</v>
-      </c>
-      <c r="AB23">
-        <v>378</v>
-      </c>
-      <c r="AC23">
-        <v>102</v>
-      </c>
-      <c r="AD23">
-        <v>636</v>
-      </c>
-      <c r="AE23">
-        <v>114</v>
       </c>
       <c r="AF23">
         <f t="shared" si="0"/>
@@ -3024,94 +3025,94 @@
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B24">
-        <v>172</v>
+        <v>884</v>
       </c>
       <c r="C24">
-        <v>538</v>
+        <v>133</v>
       </c>
       <c r="D24">
-        <v>35</v>
+        <v>343</v>
       </c>
       <c r="E24">
-        <v>441</v>
+        <v>693</v>
       </c>
       <c r="F24">
-        <v>435</v>
+        <v>863</v>
       </c>
       <c r="G24">
-        <v>119</v>
+        <v>890</v>
       </c>
       <c r="H24">
-        <v>451</v>
+        <v>887</v>
       </c>
       <c r="I24">
-        <v>766</v>
+        <v>107</v>
       </c>
       <c r="J24">
-        <v>527</v>
+        <v>540</v>
       </c>
       <c r="K24">
-        <v>23</v>
+        <v>456</v>
       </c>
       <c r="L24">
-        <v>738</v>
+        <v>287</v>
       </c>
       <c r="M24">
+        <v>786</v>
+      </c>
+      <c r="N24">
+        <v>594</v>
+      </c>
+      <c r="O24">
+        <v>328</v>
+      </c>
+      <c r="P24">
+        <v>341</v>
+      </c>
+      <c r="Q24">
+        <v>500</v>
+      </c>
+      <c r="R24">
+        <v>395</v>
+      </c>
+      <c r="S24">
+        <v>114</v>
+      </c>
+      <c r="T24">
+        <v>610</v>
+      </c>
+      <c r="U24">
+        <v>517</v>
+      </c>
+      <c r="V24">
+        <v>87</v>
+      </c>
+      <c r="W24">
+        <v>459</v>
+      </c>
+      <c r="X24">
+        <v>75</v>
+      </c>
+      <c r="Y24">
+        <v>897</v>
+      </c>
+      <c r="Z24">
+        <v>212</v>
+      </c>
+      <c r="AA24">
+        <v>791</v>
+      </c>
+      <c r="AB24">
+        <v>289</v>
+      </c>
+      <c r="AC24">
         <v>21</v>
       </c>
-      <c r="N24">
-        <v>302</v>
-      </c>
-      <c r="O24">
-        <v>462</v>
-      </c>
-      <c r="P24">
-        <v>774</v>
-      </c>
-      <c r="Q24">
-        <v>809</v>
-      </c>
-      <c r="R24">
-        <v>675</v>
-      </c>
-      <c r="S24">
-        <v>130</v>
-      </c>
-      <c r="T24">
-        <v>13</v>
-      </c>
-      <c r="U24">
-        <v>718</v>
-      </c>
-      <c r="V24">
-        <v>510</v>
-      </c>
-      <c r="W24">
-        <v>606</v>
-      </c>
-      <c r="X24">
-        <v>574</v>
-      </c>
-      <c r="Y24">
-        <v>780</v>
-      </c>
-      <c r="Z24">
-        <v>897</v>
-      </c>
-      <c r="AA24">
-        <v>520</v>
-      </c>
-      <c r="AB24">
-        <v>374</v>
-      </c>
-      <c r="AC24">
-        <v>84</v>
-      </c>
       <c r="AD24">
-        <v>800</v>
+        <v>118</v>
       </c>
       <c r="AE24">
-        <v>221</v>
+        <v>298</v>
       </c>
       <c r="AF24">
         <f t="shared" si="0"/>
@@ -3120,94 +3121,94 @@
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B25">
-        <v>805</v>
+        <v>572</v>
       </c>
       <c r="C25">
-        <v>60</v>
+        <v>565</v>
       </c>
       <c r="D25">
-        <v>491</v>
+        <v>374</v>
       </c>
       <c r="E25">
-        <v>148</v>
+        <v>849</v>
       </c>
       <c r="F25">
-        <v>630</v>
+        <v>396</v>
       </c>
       <c r="G25">
-        <v>572</v>
+        <v>478</v>
       </c>
       <c r="H25">
-        <v>465</v>
+        <v>783</v>
       </c>
       <c r="I25">
-        <v>400</v>
+        <v>495</v>
       </c>
       <c r="J25">
-        <v>875</v>
+        <v>74</v>
       </c>
       <c r="K25">
-        <v>74</v>
+        <v>702</v>
       </c>
       <c r="L25">
-        <v>242</v>
+        <v>755</v>
       </c>
       <c r="M25">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="N25">
-        <v>547</v>
+        <v>588</v>
       </c>
       <c r="O25">
-        <v>15</v>
+        <v>845</v>
       </c>
       <c r="P25">
-        <v>454</v>
+        <v>191</v>
       </c>
       <c r="Q25">
-        <v>240</v>
+        <v>569</v>
       </c>
       <c r="R25">
-        <v>239</v>
+        <v>185</v>
       </c>
       <c r="S25">
+        <v>384</v>
+      </c>
+      <c r="T25">
         <v>692</v>
       </c>
-      <c r="T25">
-        <v>350</v>
-      </c>
       <c r="U25">
-        <v>331</v>
+        <v>388</v>
       </c>
       <c r="V25">
-        <v>224</v>
+        <v>615</v>
       </c>
       <c r="W25">
-        <v>197</v>
+        <v>46</v>
       </c>
       <c r="X25">
-        <v>485</v>
+        <v>513</v>
       </c>
       <c r="Y25">
-        <v>797</v>
+        <v>203</v>
       </c>
       <c r="Z25">
-        <v>533</v>
+        <v>430</v>
       </c>
       <c r="AA25">
-        <v>399</v>
+        <v>368</v>
       </c>
       <c r="AB25">
-        <v>638</v>
+        <v>301</v>
       </c>
       <c r="AC25">
-        <v>697</v>
+        <v>2</v>
       </c>
       <c r="AD25">
-        <v>392</v>
+        <v>340</v>
       </c>
       <c r="AE25">
-        <v>852</v>
+        <v>163</v>
       </c>
       <c r="AF25">
         <f t="shared" si="0"/>
@@ -3216,94 +3217,94 @@
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B26">
-        <v>540</v>
+        <v>510</v>
       </c>
       <c r="C26">
-        <v>447</v>
+        <v>587</v>
       </c>
       <c r="D26">
+        <v>393</v>
+      </c>
+      <c r="E26">
+        <v>184</v>
+      </c>
+      <c r="F26">
+        <v>369</v>
+      </c>
+      <c r="G26">
+        <v>816</v>
+      </c>
+      <c r="H26">
+        <v>637</v>
+      </c>
+      <c r="I26">
+        <v>266</v>
+      </c>
+      <c r="J26">
         <v>705</v>
       </c>
-      <c r="E26">
-        <v>401</v>
-      </c>
-      <c r="F26">
-        <v>222</v>
-      </c>
-      <c r="G26">
-        <v>569</v>
-      </c>
-      <c r="H26">
-        <v>11</v>
-      </c>
-      <c r="I26">
-        <v>75</v>
-      </c>
-      <c r="J26">
-        <v>679</v>
-      </c>
       <c r="K26">
-        <v>543</v>
+        <v>676</v>
       </c>
       <c r="L26">
-        <v>560</v>
+        <v>259</v>
       </c>
       <c r="M26">
-        <v>381</v>
+        <v>549</v>
       </c>
       <c r="N26">
-        <v>644</v>
+        <v>327</v>
       </c>
       <c r="O26">
-        <v>702</v>
+        <v>564</v>
       </c>
       <c r="P26">
-        <v>56</v>
+        <v>750</v>
       </c>
       <c r="Q26">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="R26">
-        <v>517</v>
+        <v>262</v>
       </c>
       <c r="S26">
-        <v>850</v>
+        <v>206</v>
       </c>
       <c r="T26">
-        <v>681</v>
+        <v>272</v>
       </c>
       <c r="U26">
-        <v>531</v>
+        <v>195</v>
       </c>
       <c r="V26">
-        <v>432</v>
+        <v>176</v>
       </c>
       <c r="W26">
-        <v>590</v>
+        <v>685</v>
       </c>
       <c r="X26">
-        <v>545</v>
+        <v>844</v>
       </c>
       <c r="Y26">
-        <v>397</v>
+        <v>878</v>
       </c>
       <c r="Z26">
-        <v>312</v>
+        <v>140</v>
       </c>
       <c r="AA26">
-        <v>402</v>
+        <v>734</v>
       </c>
       <c r="AB26">
-        <v>33</v>
+        <v>570</v>
       </c>
       <c r="AC26">
-        <v>279</v>
+        <v>621</v>
       </c>
       <c r="AD26">
-        <v>755</v>
+        <v>188</v>
       </c>
       <c r="AE26">
-        <v>648</v>
+        <v>136</v>
       </c>
       <c r="AF26">
         <f t="shared" si="0"/>
@@ -3312,94 +3313,94 @@
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B27">
-        <v>626</v>
+        <v>197</v>
       </c>
       <c r="C27">
-        <v>514</v>
+        <v>858</v>
       </c>
       <c r="D27">
-        <v>135</v>
+        <v>826</v>
       </c>
       <c r="E27">
-        <v>550</v>
+        <v>353</v>
       </c>
       <c r="F27">
-        <v>356</v>
+        <v>121</v>
       </c>
       <c r="G27">
-        <v>431</v>
+        <v>583</v>
       </c>
       <c r="H27">
-        <v>238</v>
+        <v>38</v>
       </c>
       <c r="I27">
-        <v>100</v>
+        <v>521</v>
       </c>
       <c r="J27">
-        <v>847</v>
+        <v>470</v>
       </c>
       <c r="K27">
-        <v>110</v>
+        <v>600</v>
       </c>
       <c r="L27">
-        <v>410</v>
+        <v>99</v>
       </c>
       <c r="M27">
-        <v>16</v>
+        <v>394</v>
       </c>
       <c r="N27">
-        <v>438</v>
+        <v>732</v>
       </c>
       <c r="O27">
-        <v>621</v>
+        <v>258</v>
       </c>
       <c r="P27">
-        <v>513</v>
+        <v>363</v>
       </c>
       <c r="Q27">
-        <v>198</v>
+        <v>319</v>
       </c>
       <c r="R27">
-        <v>888</v>
+        <v>309</v>
       </c>
       <c r="S27">
-        <v>848</v>
+        <v>244</v>
       </c>
       <c r="T27">
-        <v>64</v>
+        <v>392</v>
       </c>
       <c r="U27">
-        <v>772</v>
+        <v>696</v>
       </c>
       <c r="V27">
-        <v>667</v>
+        <v>462</v>
       </c>
       <c r="W27">
-        <v>43</v>
+        <v>211</v>
       </c>
       <c r="X27">
-        <v>555</v>
+        <v>535</v>
       </c>
       <c r="Y27">
-        <v>646</v>
+        <v>727</v>
       </c>
       <c r="Z27">
-        <v>98</v>
+        <v>190</v>
       </c>
       <c r="AA27">
-        <v>611</v>
+        <v>640</v>
       </c>
       <c r="AB27">
-        <v>203</v>
+        <v>221</v>
       </c>
       <c r="AC27">
-        <v>831</v>
+        <v>799</v>
       </c>
       <c r="AD27">
-        <v>603</v>
+        <v>520</v>
       </c>
       <c r="AE27">
-        <v>583</v>
+        <v>837</v>
       </c>
       <c r="AF27">
         <f t="shared" si="0"/>
@@ -3408,94 +3409,94 @@
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B28">
-        <v>750</v>
+        <v>842</v>
       </c>
       <c r="C28">
-        <v>839</v>
+        <v>575</v>
       </c>
       <c r="D28">
-        <v>54</v>
+        <v>793</v>
       </c>
       <c r="E28">
-        <v>812</v>
+        <v>33</v>
       </c>
       <c r="F28">
-        <v>453</v>
+        <v>373</v>
       </c>
       <c r="G28">
-        <v>299</v>
+        <v>126</v>
       </c>
       <c r="H28">
-        <v>868</v>
+        <v>8</v>
       </c>
       <c r="I28">
-        <v>789</v>
+        <v>503</v>
       </c>
       <c r="J28">
-        <v>193</v>
+        <v>159</v>
       </c>
       <c r="K28">
-        <v>157</v>
+        <v>605</v>
       </c>
       <c r="L28">
-        <v>179</v>
+        <v>205</v>
       </c>
       <c r="M28">
-        <v>802</v>
+        <v>37</v>
       </c>
       <c r="N28">
-        <v>795</v>
+        <v>744</v>
       </c>
       <c r="O28">
-        <v>664</v>
+        <v>745</v>
       </c>
       <c r="P28">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="Q28">
-        <v>645</v>
+        <v>622</v>
       </c>
       <c r="R28">
-        <v>396</v>
+        <v>776</v>
       </c>
       <c r="S28">
-        <v>539</v>
+        <v>321</v>
       </c>
       <c r="T28">
-        <v>552</v>
+        <v>556</v>
       </c>
       <c r="U28">
-        <v>29</v>
+        <v>458</v>
       </c>
       <c r="V28">
-        <v>711</v>
+        <v>484</v>
       </c>
       <c r="W28">
-        <v>353</v>
+        <v>42</v>
       </c>
       <c r="X28">
-        <v>62</v>
+        <v>389</v>
       </c>
       <c r="Y28">
-        <v>262</v>
+        <v>634</v>
       </c>
       <c r="Z28">
-        <v>361</v>
+        <v>502</v>
       </c>
       <c r="AA28">
-        <v>345</v>
+        <v>544</v>
       </c>
       <c r="AB28">
-        <v>18</v>
+        <v>236</v>
       </c>
       <c r="AC28">
-        <v>858</v>
+        <v>288</v>
       </c>
       <c r="AD28">
-        <v>169</v>
+        <v>698</v>
       </c>
       <c r="AE28">
-        <v>202</v>
+        <v>862</v>
       </c>
       <c r="AF28">
         <f t="shared" si="0"/>
@@ -3504,94 +3505,94 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B29">
-        <v>357</v>
+        <v>72</v>
       </c>
       <c r="C29">
-        <v>832</v>
+        <v>14</v>
       </c>
       <c r="D29">
+        <v>125</v>
+      </c>
+      <c r="E29">
+        <v>807</v>
+      </c>
+      <c r="F29">
+        <v>43</v>
+      </c>
+      <c r="G29">
+        <v>872</v>
+      </c>
+      <c r="H29">
+        <v>160</v>
+      </c>
+      <c r="I29">
+        <v>751</v>
+      </c>
+      <c r="J29">
+        <v>467</v>
+      </c>
+      <c r="K29">
+        <v>465</v>
+      </c>
+      <c r="L29">
+        <v>562</v>
+      </c>
+      <c r="M29">
+        <v>646</v>
+      </c>
+      <c r="N29">
+        <v>213</v>
+      </c>
+      <c r="O29">
+        <v>348</v>
+      </c>
+      <c r="P29">
         <v>730</v>
       </c>
-      <c r="E29">
-        <v>759</v>
-      </c>
-      <c r="F29">
-        <v>763</v>
-      </c>
-      <c r="G29">
-        <v>657</v>
-      </c>
-      <c r="H29">
-        <v>340</v>
-      </c>
-      <c r="I29">
-        <v>241</v>
-      </c>
-      <c r="J29">
-        <v>152</v>
-      </c>
-      <c r="K29">
-        <v>409</v>
-      </c>
-      <c r="L29">
-        <v>28</v>
-      </c>
-      <c r="M29">
-        <v>865</v>
-      </c>
-      <c r="N29">
-        <v>542</v>
-      </c>
-      <c r="O29">
-        <v>316</v>
-      </c>
-      <c r="P29">
-        <v>237</v>
-      </c>
       <c r="Q29">
-        <v>585</v>
+        <v>805</v>
       </c>
       <c r="R29">
-        <v>522</v>
+        <v>231</v>
       </c>
       <c r="S29">
-        <v>628</v>
+        <v>723</v>
       </c>
       <c r="T29">
-        <v>364</v>
+        <v>533</v>
       </c>
       <c r="U29">
-        <v>803</v>
+        <v>888</v>
       </c>
       <c r="V29">
+        <v>10</v>
+      </c>
+      <c r="W29">
+        <v>704</v>
+      </c>
+      <c r="X29">
+        <v>577</v>
+      </c>
+      <c r="Y29">
+        <v>25</v>
+      </c>
+      <c r="Z29">
+        <v>738</v>
+      </c>
+      <c r="AA29">
+        <v>61</v>
+      </c>
+      <c r="AB29">
+        <v>900</v>
+      </c>
+      <c r="AC29">
         <v>6</v>
       </c>
-      <c r="W29">
-        <v>57</v>
-      </c>
-      <c r="X29">
-        <v>792</v>
-      </c>
-      <c r="Y29">
-        <v>26</v>
-      </c>
-      <c r="Z29">
-        <v>273</v>
-      </c>
-      <c r="AA29">
-        <v>704</v>
-      </c>
-      <c r="AB29">
-        <v>614</v>
-      </c>
-      <c r="AC29">
-        <v>232</v>
-      </c>
       <c r="AD29">
-        <v>113</v>
+        <v>141</v>
       </c>
       <c r="AE29">
-        <v>568</v>
+        <v>898</v>
       </c>
       <c r="AF29">
         <f t="shared" si="0"/>
@@ -3600,94 +3601,94 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.2">
       <c r="B30">
+        <v>868</v>
+      </c>
+      <c r="C30">
+        <v>116</v>
+      </c>
+      <c r="D30">
+        <v>471</v>
+      </c>
+      <c r="E30">
+        <v>57</v>
+      </c>
+      <c r="F30">
+        <v>5</v>
+      </c>
+      <c r="G30">
+        <v>127</v>
+      </c>
+      <c r="H30">
+        <v>833</v>
+      </c>
+      <c r="I30">
+        <v>96</v>
+      </c>
+      <c r="J30">
+        <v>69</v>
+      </c>
+      <c r="K30">
+        <v>443</v>
+      </c>
+      <c r="L30">
+        <v>362</v>
+      </c>
+      <c r="M30">
+        <v>73</v>
+      </c>
+      <c r="N30">
+        <v>410</v>
+      </c>
+      <c r="O30">
+        <v>4</v>
+      </c>
+      <c r="P30">
+        <v>665</v>
+      </c>
+      <c r="Q30">
+        <v>337</v>
+      </c>
+      <c r="R30">
+        <v>611</v>
+      </c>
+      <c r="S30">
+        <v>899</v>
+      </c>
+      <c r="T30">
+        <v>385</v>
+      </c>
+      <c r="U30">
+        <v>496</v>
+      </c>
+      <c r="V30">
+        <v>804</v>
+      </c>
+      <c r="W30">
+        <v>438</v>
+      </c>
+      <c r="X30">
+        <v>825</v>
+      </c>
+      <c r="Y30">
+        <v>635</v>
+      </c>
+      <c r="Z30">
+        <v>873</v>
+      </c>
+      <c r="AA30">
+        <v>748</v>
+      </c>
+      <c r="AB30">
+        <v>273</v>
+      </c>
+      <c r="AC30">
+        <v>153</v>
+      </c>
+      <c r="AD30">
+        <v>880</v>
+      </c>
+      <c r="AE30">
         <v>559</v>
-      </c>
-      <c r="C30">
-        <v>360</v>
-      </c>
-      <c r="D30">
-        <v>450</v>
-      </c>
-      <c r="E30">
-        <v>45</v>
-      </c>
-      <c r="F30">
-        <v>677</v>
-      </c>
-      <c r="G30">
-        <v>430</v>
-      </c>
-      <c r="H30">
-        <v>694</v>
-      </c>
-      <c r="I30">
-        <v>725</v>
-      </c>
-      <c r="J30">
-        <v>171</v>
-      </c>
-      <c r="K30">
-        <v>177</v>
-      </c>
-      <c r="L30">
-        <v>133</v>
-      </c>
-      <c r="M30">
-        <v>229</v>
-      </c>
-      <c r="N30">
-        <v>276</v>
-      </c>
-      <c r="O30">
-        <v>736</v>
-      </c>
-      <c r="P30">
-        <v>63</v>
-      </c>
-      <c r="Q30">
-        <v>315</v>
-      </c>
-      <c r="R30">
-        <v>117</v>
-      </c>
-      <c r="S30">
-        <v>120</v>
-      </c>
-      <c r="T30">
-        <v>854</v>
-      </c>
-      <c r="U30">
-        <v>883</v>
-      </c>
-      <c r="V30">
-        <v>726</v>
-      </c>
-      <c r="W30">
-        <v>296</v>
-      </c>
-      <c r="X30">
-        <v>82</v>
-      </c>
-      <c r="Y30">
-        <v>864</v>
-      </c>
-      <c r="Z30">
-        <v>685</v>
-      </c>
-      <c r="AA30">
-        <v>661</v>
-      </c>
-      <c r="AB30">
-        <v>342</v>
-      </c>
-      <c r="AC30">
-        <v>799</v>
-      </c>
-      <c r="AD30">
-        <v>233</v>
-      </c>
-      <c r="AE30">
-        <v>813</v>
       </c>
       <c r="AF30">
         <f t="shared" si="0"/>
@@ -3697,7 +3698,7 @@
     <row r="31" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A31">
         <f>SUM(B30,C29,D28,E27,F26,G25,H24,I23,J22,K21,L20,M19,N18,O17,P16,Q15,R14,S13,T12,U11,V10,W9,X8,Y7,Z6,AA5,AB4,AC3,AD2,AE1)</f>
-        <v>13515</v>
+        <v>16390</v>
       </c>
       <c r="B31">
         <f>SUM(B1:B30)</f>

</xml_diff>

<commit_message>
Prefer to pass Evolutions a starter Magic rather than specifying an order value
</commit_message>
<xml_diff>
--- a/examples/magic-checker.xlsx
+++ b/examples/magic-checker.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lioudt/Documents/Projects/Albrecht/examples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD58C7B-462F-C540-BD90-5064EC2C64F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76E22C9C-3C82-8C44-8F8D-035ABEF12D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42740" yWindow="1820" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{88018936-75B0-5E47-B04F-69E20E6F83B4}"/>
+    <workbookView xWindow="42740" yWindow="1820" windowWidth="28040" windowHeight="17440" xr2:uid="{88018936-75B0-5E47-B04F-69E20E6F83B4}"/>
   </bookViews>
   <sheets>
-    <sheet name="9" sheetId="1" r:id="rId1"/>
-    <sheet name="30" sheetId="2" r:id="rId2"/>
+    <sheet name="8" sheetId="3" r:id="rId1"/>
+    <sheet name="9" sheetId="1" r:id="rId2"/>
+    <sheet name="30" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,7 +72,67 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="10">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -421,6 +482,319 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9341CC-8395-3F4F-A03C-E334D2D0741A}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>12</v>
+      </c>
+      <c r="C1">
+        <v>31</v>
+      </c>
+      <c r="D1">
+        <v>60</v>
+      </c>
+      <c r="E1">
+        <v>33</v>
+      </c>
+      <c r="F1">
+        <v>30</v>
+      </c>
+      <c r="G1">
+        <v>35</v>
+      </c>
+      <c r="H1">
+        <v>39</v>
+      </c>
+      <c r="I1">
+        <v>20</v>
+      </c>
+      <c r="J1">
+        <f>SUM(B1:I1)</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>62</v>
+      </c>
+      <c r="C2">
+        <v>32</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>38</v>
+      </c>
+      <c r="F2">
+        <v>21</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>44</v>
+      </c>
+      <c r="I2">
+        <v>40</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J8" si="0">SUM(B2:I2)</f>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>23</v>
+      </c>
+      <c r="C3">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>43</v>
+      </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
+      <c r="G3">
+        <v>51</v>
+      </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>58</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>25</v>
+      </c>
+      <c r="C4">
+        <v>18</v>
+      </c>
+      <c r="D4">
+        <v>34</v>
+      </c>
+      <c r="E4">
+        <v>48</v>
+      </c>
+      <c r="F4">
+        <v>8</v>
+      </c>
+      <c r="G4">
+        <v>27</v>
+      </c>
+      <c r="H4">
+        <v>54</v>
+      </c>
+      <c r="I4">
+        <v>46</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>45</v>
+      </c>
+      <c r="E5">
+        <v>56</v>
+      </c>
+      <c r="F5">
+        <v>49</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>36</v>
+      </c>
+      <c r="I5">
+        <v>26</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>53</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>17</v>
+      </c>
+      <c r="F6">
+        <v>63</v>
+      </c>
+      <c r="G6">
+        <v>55</v>
+      </c>
+      <c r="H6">
+        <v>61</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>64</v>
+      </c>
+      <c r="C7">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>24</v>
+      </c>
+      <c r="E7">
+        <v>15</v>
+      </c>
+      <c r="F7">
+        <v>19</v>
+      </c>
+      <c r="G7">
+        <v>22</v>
+      </c>
+      <c r="H7">
+        <v>14</v>
+      </c>
+      <c r="I7">
+        <v>52</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>29</v>
+      </c>
+      <c r="C8">
+        <v>47</v>
+      </c>
+      <c r="D8">
+        <v>42</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>59</v>
+      </c>
+      <c r="G8">
+        <v>57</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>13</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <f>SUM(B8,C7,D6,E5,F4,G3,H2,I1)</f>
+        <v>260</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B1:B8)</f>
+        <v>260</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:I9" si="1">SUM(C1:C8)</f>
+        <v>260</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>260</v>
+      </c>
+      <c r="J9">
+        <f>SUM(B1,C2,D3,E4,F5,G6,H7,I8)</f>
+        <v>260</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A9:J9">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>260</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="notEqual">
+      <formula>260</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J8">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>260</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
+      <formula>260</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D268AA-9B72-C74E-AFE5-98BDA6ADCB5F}">
   <dimension ref="A1:K10"/>
   <sheetViews>
@@ -775,10 +1149,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A10:K10 K1:K9">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="notEqual">
       <formula>369</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>369</formula>
     </cfRule>
   </conditionalFormatting>
@@ -787,11 +1161,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E8CD7C-B77D-014B-894F-5F39F26D2D1B}">
   <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0"/>
+    <sheetView zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -3807,10 +4183,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A31:AF31 AF1:AF30">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>13515</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="1" operator="notEqual">
       <formula>13515</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>